<commit_message>
versions updated with results
</commit_message>
<xml_diff>
--- a/stats/stats.xlsx
+++ b/stats/stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ng vs em" sheetId="2" r:id="rId1"/>
@@ -77,8 +77,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -89,13 +91,15 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -148,7 +152,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>all!$B$1</c:f>
+              <c:f>'ng vs em'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -160,10 +164,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>all!$A$2:$A$21</c:f>
+              <c:f>'ng vs em'!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>100.0</c:v>
                 </c:pt>
@@ -223,75 +227,105 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all!$B$2:$B$21</c:f>
+              <c:f>'ng vs em'!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>2.586</c:v>
+                  <c:v>1.864</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.293</c:v>
+                  <c:v>5.165</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.829</c:v>
+                  <c:v>9.862</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.728</c:v>
+                  <c:v>16.056</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.663</c:v>
+                  <c:v>23.82</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.152</c:v>
+                  <c:v>33.012</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.791</c:v>
+                  <c:v>43.935</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>73.449</c:v>
+                  <c:v>56.26</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89.715</c:v>
+                  <c:v>70.545</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>92.629</c:v>
+                  <c:v>85.947</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>112.34</c:v>
+                  <c:v>103.97</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>130.63</c:v>
+                  <c:v>124.785</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>152.316</c:v>
+                  <c:v>147.365</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>177.452</c:v>
+                  <c:v>184.287</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>202.935</c:v>
+                  <c:v>225.7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>232.102</c:v>
+                  <c:v>270.585</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>262.41</c:v>
+                  <c:v>319.389</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>298.721</c:v>
+                  <c:v>371.258</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>327.525</c:v>
+                  <c:v>427.328</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>363.817</c:v>
+                  <c:v>486.441</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>550.503</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>617.864</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>689.884</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>766.121</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>845.238</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -302,7 +336,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>all!$C$1</c:f>
+              <c:f>'ng vs em'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -314,10 +348,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>all!$A$2:$A$21</c:f>
+              <c:f>'ng vs em'!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>100.0</c:v>
                 </c:pt>
@@ -377,75 +411,105 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all!$C$2:$C$21</c:f>
+              <c:f>'ng vs em'!$C$2:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>2.494</c:v>
+                  <c:v>1.697</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.807</c:v>
+                  <c:v>4.171</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.053</c:v>
+                  <c:v>9.384</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.966</c:v>
+                  <c:v>16.485</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.114</c:v>
+                  <c:v>25.624</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.619</c:v>
+                  <c:v>35.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.578</c:v>
+                  <c:v>47.327</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41.08</c:v>
+                  <c:v>60.307</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>48.468</c:v>
+                  <c:v>74.843</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>56.157</c:v>
+                  <c:v>90.887</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>64.828</c:v>
+                  <c:v>108.644</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>74.05</c:v>
+                  <c:v>127.982</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>84.296</c:v>
+                  <c:v>148.795</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>95.065</c:v>
+                  <c:v>171.292</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>105.575</c:v>
+                  <c:v>195.719</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>117.583</c:v>
+                  <c:v>221.306</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>132.729</c:v>
+                  <c:v>248.447</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>145.749</c:v>
+                  <c:v>277.07</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>160.564</c:v>
+                  <c:v>307.691</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>174.463</c:v>
+                  <c:v>339.419</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>372.743</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>407.828</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>444.496</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>482.947</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>522.631</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -461,11 +525,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="2111286952"/>
-        <c:axId val="2111289928"/>
+        <c:axId val="-2144108664"/>
+        <c:axId val="-2143991384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2111286952"/>
+        <c:axId val="-2144108664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -475,7 +539,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111289928"/>
+        <c:crossAx val="-2143991384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -483,7 +547,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2111289928"/>
+        <c:axId val="-2143991384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,7 +558,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111286952"/>
+        <c:crossAx val="-2144108664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -541,11 +605,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Angular</a:t>
+              <a:t>Angular vs.</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs. Ember</a:t>
+              <a:t> Ember</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -565,7 +629,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>all!$B$1</c:f>
+              <c:f>'ng vs em'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -579,10 +643,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>all!$A$2:$A$21</c:f>
+              <c:f>'ng vs em'!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>100.0</c:v>
                 </c:pt>
@@ -642,75 +706,105 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all!$B$2:$B$21</c:f>
+              <c:f>'ng vs em'!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>2.586</c:v>
+                  <c:v>1.864</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.293</c:v>
+                  <c:v>5.165</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.829</c:v>
+                  <c:v>9.862</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.728</c:v>
+                  <c:v>16.056</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.663</c:v>
+                  <c:v>23.82</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.152</c:v>
+                  <c:v>33.012</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.791</c:v>
+                  <c:v>43.935</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>73.449</c:v>
+                  <c:v>56.26</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89.715</c:v>
+                  <c:v>70.545</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>92.629</c:v>
+                  <c:v>85.947</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>112.34</c:v>
+                  <c:v>103.97</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>130.63</c:v>
+                  <c:v>124.785</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>152.316</c:v>
+                  <c:v>147.365</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>177.452</c:v>
+                  <c:v>184.287</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>202.935</c:v>
+                  <c:v>225.7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>232.102</c:v>
+                  <c:v>270.585</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>262.41</c:v>
+                  <c:v>319.389</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>298.721</c:v>
+                  <c:v>371.258</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>327.525</c:v>
+                  <c:v>427.328</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>363.817</c:v>
+                  <c:v>486.441</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>550.503</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>617.864</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>689.884</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>766.121</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>845.238</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -722,7 +816,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>all!$C$1</c:f>
+              <c:f>'ng vs em'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -736,10 +830,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>all!$A$2:$A$21</c:f>
+              <c:f>'ng vs em'!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>100.0</c:v>
                 </c:pt>
@@ -799,75 +893,105 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all!$C$2:$C$21</c:f>
+              <c:f>'ng vs em'!$C$2:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>2.494</c:v>
+                  <c:v>1.697</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.807</c:v>
+                  <c:v>4.171</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.053</c:v>
+                  <c:v>9.384</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.966</c:v>
+                  <c:v>16.485</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.114</c:v>
+                  <c:v>25.624</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.619</c:v>
+                  <c:v>35.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.578</c:v>
+                  <c:v>47.327</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41.08</c:v>
+                  <c:v>60.307</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>48.468</c:v>
+                  <c:v>74.843</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>56.157</c:v>
+                  <c:v>90.887</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>64.828</c:v>
+                  <c:v>108.644</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>74.05</c:v>
+                  <c:v>127.982</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>84.296</c:v>
+                  <c:v>148.795</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>95.065</c:v>
+                  <c:v>171.292</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>105.575</c:v>
+                  <c:v>195.719</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>117.583</c:v>
+                  <c:v>221.306</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>132.729</c:v>
+                  <c:v>248.447</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>145.749</c:v>
+                  <c:v>277.07</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>160.564</c:v>
+                  <c:v>307.691</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>174.463</c:v>
+                  <c:v>339.419</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>372.743</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>407.828</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>444.496</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>482.947</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>522.631</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -884,11 +1008,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2111362008"/>
-        <c:axId val="2111364984"/>
+        <c:axId val="-2144854104"/>
+        <c:axId val="-2144869624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2111362008"/>
+        <c:axId val="-2144854104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,7 +1022,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111364984"/>
+        <c:crossAx val="-2144869624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -906,43 +1030,29 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2111364984"/>
+        <c:axId val="-2144869624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>seconds</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111362008"/>
+        <c:spPr>
+          <a:ln w="9525">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="-2144854104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -988,6 +1098,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1014,10 +1125,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>all!$A$2:$A$21</c:f>
+              <c:f>all!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>100.0</c:v>
                 </c:pt>
@@ -1077,75 +1188,105 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all!$B$2:$B$21</c:f>
+              <c:f>all!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>2.586</c:v>
+                  <c:v>1.864</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.293</c:v>
+                  <c:v>5.165</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.829</c:v>
+                  <c:v>9.862</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.728</c:v>
+                  <c:v>16.056</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.663</c:v>
+                  <c:v>23.82</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.152</c:v>
+                  <c:v>33.012</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.791</c:v>
+                  <c:v>43.935</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>73.449</c:v>
+                  <c:v>56.26</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89.715</c:v>
+                  <c:v>70.545</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>92.629</c:v>
+                  <c:v>85.947</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>112.34</c:v>
+                  <c:v>103.97</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>130.63</c:v>
+                  <c:v>124.785</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>152.316</c:v>
+                  <c:v>147.365</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>177.452</c:v>
+                  <c:v>184.287</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>202.935</c:v>
+                  <c:v>225.7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>232.102</c:v>
+                  <c:v>270.585</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>262.41</c:v>
+                  <c:v>319.389</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>298.721</c:v>
+                  <c:v>371.258</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>327.525</c:v>
+                  <c:v>427.328</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>363.817</c:v>
+                  <c:v>486.441</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>550.503</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>617.864</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>689.884</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>766.121</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>845.238</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1168,10 +1309,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>all!$A$2:$A$21</c:f>
+              <c:f>all!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>100.0</c:v>
                 </c:pt>
@@ -1231,75 +1372,105 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all!$C$2:$C$21</c:f>
+              <c:f>all!$C$2:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>2.494</c:v>
+                  <c:v>1.697</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.807</c:v>
+                  <c:v>4.171</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.053</c:v>
+                  <c:v>9.384</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.966</c:v>
+                  <c:v>16.485</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.114</c:v>
+                  <c:v>25.624</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.619</c:v>
+                  <c:v>35.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.578</c:v>
+                  <c:v>47.327</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41.08</c:v>
+                  <c:v>60.307</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>48.468</c:v>
+                  <c:v>74.843</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>56.157</c:v>
+                  <c:v>90.887</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>64.828</c:v>
+                  <c:v>108.644</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>74.05</c:v>
+                  <c:v>127.982</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>84.296</c:v>
+                  <c:v>148.795</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>95.065</c:v>
+                  <c:v>171.292</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>105.575</c:v>
+                  <c:v>195.719</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>117.583</c:v>
+                  <c:v>221.306</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>132.729</c:v>
+                  <c:v>248.447</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>145.749</c:v>
+                  <c:v>277.07</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>160.564</c:v>
+                  <c:v>307.691</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>174.463</c:v>
+                  <c:v>339.419</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>372.743</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>407.828</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>444.496</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>482.947</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>522.631</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1322,10 +1493,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>all!$A$2:$A$21</c:f>
+              <c:f>all!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>100.0</c:v>
                 </c:pt>
@@ -1385,75 +1556,105 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all!$D$2:$D$21</c:f>
+              <c:f>all!$D$2:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>1.878</c:v>
+                  <c:v>1.516</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.801</c:v>
+                  <c:v>3.195</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.159</c:v>
+                  <c:v>5.611</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.32</c:v>
+                  <c:v>8.846</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.929</c:v>
+                  <c:v>12.412</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.993</c:v>
+                  <c:v>16.482</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.4</c:v>
+                  <c:v>21.008</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33.35</c:v>
+                  <c:v>26.078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.175</c:v>
+                  <c:v>31.578</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>47.644</c:v>
+                  <c:v>37.593</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55.583</c:v>
+                  <c:v>44.136</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>63.031</c:v>
+                  <c:v>51.371</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>71.541</c:v>
+                  <c:v>58.686</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>80.123</c:v>
+                  <c:v>66.471</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>89.67400000000001</c:v>
+                  <c:v>74.462</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>99.66</c:v>
+                  <c:v>83.539</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>110.457</c:v>
+                  <c:v>93.1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>120.449</c:v>
+                  <c:v>102.709</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>135.153</c:v>
+                  <c:v>112.867</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>174.677</c:v>
+                  <c:v>133.6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>167.341</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>202.888</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>240.468</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>279.328</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>319.846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1469,11 +1670,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="2111416696"/>
-        <c:axId val="2111419672"/>
+        <c:axId val="2086475784"/>
+        <c:axId val="2086478760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2111416696"/>
+        <c:axId val="2086475784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1483,7 +1684,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111419672"/>
+        <c:crossAx val="2086478760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1491,7 +1692,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2111419672"/>
+        <c:axId val="2086478760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1502,13 +1703,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111416696"/>
+        <c:crossAx val="2086475784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1553,6 +1755,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1580,10 +1783,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>all!$A$2:$A$21</c:f>
+              <c:f>all!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>100.0</c:v>
                 </c:pt>
@@ -1643,75 +1846,105 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all!$B$2:$B$21</c:f>
+              <c:f>all!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>2.586</c:v>
+                  <c:v>1.864</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.293</c:v>
+                  <c:v>5.165</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.829</c:v>
+                  <c:v>9.862</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.728</c:v>
+                  <c:v>16.056</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.663</c:v>
+                  <c:v>23.82</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.152</c:v>
+                  <c:v>33.012</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.791</c:v>
+                  <c:v>43.935</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>73.449</c:v>
+                  <c:v>56.26</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89.715</c:v>
+                  <c:v>70.545</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>92.629</c:v>
+                  <c:v>85.947</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>112.34</c:v>
+                  <c:v>103.97</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>130.63</c:v>
+                  <c:v>124.785</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>152.316</c:v>
+                  <c:v>147.365</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>177.452</c:v>
+                  <c:v>184.287</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>202.935</c:v>
+                  <c:v>225.7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>232.102</c:v>
+                  <c:v>270.585</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>262.41</c:v>
+                  <c:v>319.389</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>298.721</c:v>
+                  <c:v>371.258</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>327.525</c:v>
+                  <c:v>427.328</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>363.817</c:v>
+                  <c:v>486.441</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>550.503</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>617.864</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>689.884</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>766.121</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>845.238</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1737,10 +1970,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>all!$A$2:$A$21</c:f>
+              <c:f>all!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>100.0</c:v>
                 </c:pt>
@@ -1800,75 +2033,105 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all!$C$2:$C$21</c:f>
+              <c:f>all!$C$2:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>2.494</c:v>
+                  <c:v>1.697</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.807</c:v>
+                  <c:v>4.171</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.053</c:v>
+                  <c:v>9.384</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.966</c:v>
+                  <c:v>16.485</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.114</c:v>
+                  <c:v>25.624</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.619</c:v>
+                  <c:v>35.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.578</c:v>
+                  <c:v>47.327</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41.08</c:v>
+                  <c:v>60.307</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>48.468</c:v>
+                  <c:v>74.843</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>56.157</c:v>
+                  <c:v>90.887</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>64.828</c:v>
+                  <c:v>108.644</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>74.05</c:v>
+                  <c:v>127.982</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>84.296</c:v>
+                  <c:v>148.795</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>95.065</c:v>
+                  <c:v>171.292</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>105.575</c:v>
+                  <c:v>195.719</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>117.583</c:v>
+                  <c:v>221.306</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>132.729</c:v>
+                  <c:v>248.447</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>145.749</c:v>
+                  <c:v>277.07</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>160.564</c:v>
+                  <c:v>307.691</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>174.463</c:v>
+                  <c:v>339.419</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>372.743</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>407.828</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>444.496</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>482.947</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>522.631</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1894,10 +2157,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>all!$A$2:$A$21</c:f>
+              <c:f>all!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>100.0</c:v>
                 </c:pt>
@@ -1957,75 +2220,105 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all!$D$2:$D$21</c:f>
+              <c:f>all!$D$2:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>1.878</c:v>
+                  <c:v>1.516</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.801</c:v>
+                  <c:v>3.195</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.159</c:v>
+                  <c:v>5.611</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.32</c:v>
+                  <c:v>8.846</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.929</c:v>
+                  <c:v>12.412</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.993</c:v>
+                  <c:v>16.482</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.4</c:v>
+                  <c:v>21.008</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33.35</c:v>
+                  <c:v>26.078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.175</c:v>
+                  <c:v>31.578</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>47.644</c:v>
+                  <c:v>37.593</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55.583</c:v>
+                  <c:v>44.136</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>63.031</c:v>
+                  <c:v>51.371</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>71.541</c:v>
+                  <c:v>58.686</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>80.123</c:v>
+                  <c:v>66.471</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>89.67400000000001</c:v>
+                  <c:v>74.462</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>99.66</c:v>
+                  <c:v>83.539</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>110.457</c:v>
+                  <c:v>93.1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>120.449</c:v>
+                  <c:v>102.709</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>135.153</c:v>
+                  <c:v>112.867</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>174.677</c:v>
+                  <c:v>133.6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>167.341</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>202.888</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>240.468</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>279.328</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>319.846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2042,11 +2335,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2111455272"/>
-        <c:axId val="2111458248"/>
+        <c:axId val="2086514584"/>
+        <c:axId val="2086517560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2111455272"/>
+        <c:axId val="2086514584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2056,7 +2349,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111458248"/>
+        <c:crossAx val="2086517560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2064,42 +2357,30 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2111458248"/>
+        <c:axId val="2086517560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>seconds</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111455272"/>
+        <c:spPr>
+          <a:ln w="9525">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="2086514584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2118,23 +2399,21 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2152,21 +2431,19 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2570,10 +2847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView showRuler="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2594,10 +2871,10 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <v>2.5859999999999999</v>
+        <v>1.8640000000000001</v>
       </c>
       <c r="C2">
-        <v>2.4940000000000002</v>
+        <v>1.6970000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2606,10 +2883,10 @@
         <v>200</v>
       </c>
       <c r="B3">
-        <v>6.2930000000000001</v>
+        <v>5.165</v>
       </c>
       <c r="C3">
-        <v>5.8070000000000004</v>
+        <v>4.1710000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2618,10 +2895,10 @@
         <v>300</v>
       </c>
       <c r="B4">
-        <v>11.829000000000001</v>
+        <v>9.8620000000000001</v>
       </c>
       <c r="C4">
-        <v>10.053000000000001</v>
+        <v>9.3840000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2630,10 +2907,10 @@
         <v>400</v>
       </c>
       <c r="B5">
-        <v>18.728000000000002</v>
+        <v>16.056000000000001</v>
       </c>
       <c r="C5">
-        <v>14.965999999999999</v>
+        <v>16.484999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2642,10 +2919,10 @@
         <v>500</v>
       </c>
       <c r="B6">
-        <v>27.663</v>
+        <v>23.82</v>
       </c>
       <c r="C6">
-        <v>20.114000000000001</v>
+        <v>25.623999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2654,10 +2931,10 @@
         <v>600</v>
       </c>
       <c r="B7">
-        <v>37.152000000000001</v>
+        <v>33.012</v>
       </c>
       <c r="C7">
-        <v>26.619</v>
+        <v>35.6</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2666,10 +2943,10 @@
         <v>700</v>
       </c>
       <c r="B8">
-        <v>57.790999999999997</v>
+        <v>43.935000000000002</v>
       </c>
       <c r="C8">
-        <v>33.578000000000003</v>
+        <v>47.326999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2678,10 +2955,10 @@
         <v>800</v>
       </c>
       <c r="B9">
-        <v>73.448999999999998</v>
+        <v>56.26</v>
       </c>
       <c r="C9">
-        <v>41.08</v>
+        <v>60.307000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2690,10 +2967,10 @@
         <v>900</v>
       </c>
       <c r="B10">
-        <v>89.715000000000003</v>
+        <v>70.545000000000002</v>
       </c>
       <c r="C10">
-        <v>48.468000000000004</v>
+        <v>74.843000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2702,10 +2979,10 @@
         <v>1000</v>
       </c>
       <c r="B11">
-        <v>92.629000000000005</v>
+        <v>85.947000000000003</v>
       </c>
       <c r="C11">
-        <v>56.156999999999996</v>
+        <v>90.887</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2714,10 +2991,10 @@
         <v>1100</v>
       </c>
       <c r="B12">
-        <v>112.34</v>
+        <v>103.97</v>
       </c>
       <c r="C12">
-        <v>64.828000000000003</v>
+        <v>108.64400000000001</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2726,10 +3003,10 @@
         <v>1200</v>
       </c>
       <c r="B13">
-        <v>130.63</v>
+        <v>124.785</v>
       </c>
       <c r="C13">
-        <v>74.05</v>
+        <v>127.982</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2738,10 +3015,10 @@
         <v>1300</v>
       </c>
       <c r="B14">
-        <v>152.316</v>
+        <v>147.36500000000001</v>
       </c>
       <c r="C14">
-        <v>84.296000000000006</v>
+        <v>148.79499999999999</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2750,10 +3027,10 @@
         <v>1400</v>
       </c>
       <c r="B15">
-        <v>177.452</v>
+        <v>184.28700000000001</v>
       </c>
       <c r="C15">
-        <v>95.064999999999998</v>
+        <v>171.292</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2762,10 +3039,10 @@
         <v>1500</v>
       </c>
       <c r="B16">
-        <v>202.935</v>
+        <v>225.7</v>
       </c>
       <c r="C16">
-        <v>105.575</v>
+        <v>195.71899999999999</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2774,10 +3051,10 @@
         <v>1600</v>
       </c>
       <c r="B17">
-        <v>232.102</v>
+        <v>270.58499999999998</v>
       </c>
       <c r="C17">
-        <v>117.583</v>
+        <v>221.30600000000001</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2786,10 +3063,10 @@
         <v>1700</v>
       </c>
       <c r="B18">
-        <v>262.41000000000003</v>
+        <v>319.38900000000001</v>
       </c>
       <c r="C18">
-        <v>132.72900000000001</v>
+        <v>248.447</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2798,10 +3075,10 @@
         <v>1800</v>
       </c>
       <c r="B19">
-        <v>298.721</v>
+        <v>371.25799999999998</v>
       </c>
       <c r="C19">
-        <v>145.749</v>
+        <v>277.07</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2810,10 +3087,10 @@
         <v>1900</v>
       </c>
       <c r="B20">
-        <v>327.52499999999998</v>
+        <v>427.32799999999997</v>
       </c>
       <c r="C20">
-        <v>160.56399999999999</v>
+        <v>307.69099999999997</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2822,14 +3099,75 @@
         <v>2000</v>
       </c>
       <c r="B21">
-        <v>363.81700000000001</v>
+        <v>486.44099999999997</v>
       </c>
       <c r="C21">
-        <v>174.46299999999999</v>
+        <v>339.41899999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <f t="shared" ref="A22:A26" si="1">$A21 + 100</f>
+        <v>2100</v>
+      </c>
+      <c r="B22">
+        <v>550.50300000000004</v>
+      </c>
+      <c r="C22">
+        <v>372.74299999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+      <c r="B23">
+        <v>617.86400000000003</v>
+      </c>
+      <c r="C23">
+        <v>407.82799999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>2300</v>
+      </c>
+      <c r="B24">
+        <v>689.88400000000001</v>
+      </c>
+      <c r="C24">
+        <v>444.49599999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>2400</v>
+      </c>
+      <c r="B25">
+        <v>766.12099999999998</v>
+      </c>
+      <c r="C25">
+        <v>482.947</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>2500</v>
+      </c>
+      <c r="B26">
+        <v>845.23800000000006</v>
+      </c>
+      <c r="C26">
+        <v>522.63099999999997</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2841,10 +3179,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2868,13 +3206,13 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <v>2.5859999999999999</v>
+        <v>1.8640000000000001</v>
       </c>
       <c r="C2">
-        <v>2.4940000000000002</v>
+        <v>1.6970000000000001</v>
       </c>
       <c r="D2">
-        <v>1.8779999999999999</v>
+        <v>1.516</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2883,13 +3221,13 @@
         <v>200</v>
       </c>
       <c r="B3">
-        <v>6.2930000000000001</v>
+        <v>5.165</v>
       </c>
       <c r="C3">
-        <v>5.8070000000000004</v>
+        <v>4.1710000000000003</v>
       </c>
       <c r="D3">
-        <v>4.8010000000000002</v>
+        <v>3.1949999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2898,13 +3236,13 @@
         <v>300</v>
       </c>
       <c r="B4">
-        <v>11.829000000000001</v>
+        <v>9.8620000000000001</v>
       </c>
       <c r="C4">
-        <v>10.053000000000001</v>
+        <v>9.3840000000000003</v>
       </c>
       <c r="D4">
-        <v>8.1590000000000007</v>
+        <v>5.6109999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2913,13 +3251,13 @@
         <v>400</v>
       </c>
       <c r="B5">
-        <v>18.728000000000002</v>
+        <v>16.056000000000001</v>
       </c>
       <c r="C5">
-        <v>14.965999999999999</v>
+        <v>16.484999999999999</v>
       </c>
       <c r="D5">
-        <v>12.32</v>
+        <v>8.8460000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2928,13 +3266,13 @@
         <v>500</v>
       </c>
       <c r="B6">
-        <v>27.663</v>
+        <v>23.82</v>
       </c>
       <c r="C6">
-        <v>20.114000000000001</v>
+        <v>25.623999999999999</v>
       </c>
       <c r="D6">
-        <v>16.928999999999998</v>
+        <v>12.412000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2943,13 +3281,13 @@
         <v>600</v>
       </c>
       <c r="B7">
-        <v>37.152000000000001</v>
+        <v>33.012</v>
       </c>
       <c r="C7">
-        <v>26.619</v>
+        <v>35.6</v>
       </c>
       <c r="D7">
-        <v>21.992999999999999</v>
+        <v>16.481999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2958,13 +3296,13 @@
         <v>700</v>
       </c>
       <c r="B8">
-        <v>57.790999999999997</v>
+        <v>43.935000000000002</v>
       </c>
       <c r="C8">
-        <v>33.578000000000003</v>
+        <v>47.326999999999998</v>
       </c>
       <c r="D8">
-        <v>27.4</v>
+        <v>21.007999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2973,13 +3311,13 @@
         <v>800</v>
       </c>
       <c r="B9">
-        <v>73.448999999999998</v>
+        <v>56.26</v>
       </c>
       <c r="C9">
-        <v>41.08</v>
+        <v>60.307000000000002</v>
       </c>
       <c r="D9">
-        <v>33.35</v>
+        <v>26.077999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2988,13 +3326,13 @@
         <v>900</v>
       </c>
       <c r="B10">
-        <v>89.715000000000003</v>
+        <v>70.545000000000002</v>
       </c>
       <c r="C10">
-        <v>48.468000000000004</v>
+        <v>74.843000000000004</v>
       </c>
       <c r="D10">
-        <v>40.174999999999997</v>
+        <v>31.577999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3003,13 +3341,13 @@
         <v>1000</v>
       </c>
       <c r="B11">
-        <v>92.629000000000005</v>
+        <v>85.947000000000003</v>
       </c>
       <c r="C11">
-        <v>56.156999999999996</v>
+        <v>90.887</v>
       </c>
       <c r="D11">
-        <v>47.643999999999998</v>
+        <v>37.593000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3018,13 +3356,13 @@
         <v>1100</v>
       </c>
       <c r="B12">
-        <v>112.34</v>
+        <v>103.97</v>
       </c>
       <c r="C12">
-        <v>64.828000000000003</v>
+        <v>108.64400000000001</v>
       </c>
       <c r="D12">
-        <v>55.582999999999998</v>
+        <v>44.136000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3033,13 +3371,13 @@
         <v>1200</v>
       </c>
       <c r="B13">
-        <v>130.63</v>
+        <v>124.785</v>
       </c>
       <c r="C13">
-        <v>74.05</v>
+        <v>127.982</v>
       </c>
       <c r="D13">
-        <v>63.030999999999999</v>
+        <v>51.371000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3048,13 +3386,13 @@
         <v>1300</v>
       </c>
       <c r="B14">
-        <v>152.316</v>
+        <v>147.36500000000001</v>
       </c>
       <c r="C14">
-        <v>84.296000000000006</v>
+        <v>148.79499999999999</v>
       </c>
       <c r="D14">
-        <v>71.540999999999997</v>
+        <v>58.686</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3063,13 +3401,13 @@
         <v>1400</v>
       </c>
       <c r="B15">
-        <v>177.452</v>
+        <v>184.28700000000001</v>
       </c>
       <c r="C15">
-        <v>95.064999999999998</v>
+        <v>171.292</v>
       </c>
       <c r="D15">
-        <v>80.123000000000005</v>
+        <v>66.471000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3078,13 +3416,13 @@
         <v>1500</v>
       </c>
       <c r="B16">
-        <v>202.935</v>
+        <v>225.7</v>
       </c>
       <c r="C16">
-        <v>105.575</v>
+        <v>195.71899999999999</v>
       </c>
       <c r="D16">
-        <v>89.674000000000007</v>
+        <v>74.462000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3093,13 +3431,13 @@
         <v>1600</v>
       </c>
       <c r="B17">
-        <v>232.102</v>
+        <v>270.58499999999998</v>
       </c>
       <c r="C17">
-        <v>117.583</v>
+        <v>221.30600000000001</v>
       </c>
       <c r="D17">
-        <v>99.66</v>
+        <v>83.539000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3108,13 +3446,13 @@
         <v>1700</v>
       </c>
       <c r="B18">
-        <v>262.41000000000003</v>
+        <v>319.38900000000001</v>
       </c>
       <c r="C18">
-        <v>132.72900000000001</v>
+        <v>248.447</v>
       </c>
       <c r="D18">
-        <v>110.45699999999999</v>
+        <v>93.1</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3123,13 +3461,13 @@
         <v>1800</v>
       </c>
       <c r="B19">
-        <v>298.721</v>
+        <v>371.25799999999998</v>
       </c>
       <c r="C19">
-        <v>145.749</v>
+        <v>277.07</v>
       </c>
       <c r="D19">
-        <v>120.449</v>
+        <v>102.709</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3138,13 +3476,13 @@
         <v>1900</v>
       </c>
       <c r="B20">
-        <v>327.52499999999998</v>
+        <v>427.32799999999997</v>
       </c>
       <c r="C20">
-        <v>160.56399999999999</v>
+        <v>307.69099999999997</v>
       </c>
       <c r="D20">
-        <v>135.15299999999999</v>
+        <v>112.867</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -3153,13 +3491,88 @@
         <v>2000</v>
       </c>
       <c r="B21">
-        <v>363.81700000000001</v>
+        <v>486.44099999999997</v>
       </c>
       <c r="C21">
-        <v>174.46299999999999</v>
+        <v>339.41899999999998</v>
       </c>
       <c r="D21">
-        <v>174.67699999999999</v>
+        <v>133.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <f t="shared" ref="A22:A26" si="1">$A21 + 100</f>
+        <v>2100</v>
+      </c>
+      <c r="B22">
+        <v>550.50300000000004</v>
+      </c>
+      <c r="C22">
+        <v>372.74299999999999</v>
+      </c>
+      <c r="D22">
+        <v>167.34100000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+      <c r="B23">
+        <v>617.86400000000003</v>
+      </c>
+      <c r="C23">
+        <v>407.82799999999997</v>
+      </c>
+      <c r="D23">
+        <v>202.88800000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>2300</v>
+      </c>
+      <c r="B24">
+        <v>689.88400000000001</v>
+      </c>
+      <c r="C24">
+        <v>444.49599999999998</v>
+      </c>
+      <c r="D24">
+        <v>240.46799999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>2400</v>
+      </c>
+      <c r="B25">
+        <v>766.12099999999998</v>
+      </c>
+      <c r="C25">
+        <v>482.947</v>
+      </c>
+      <c r="D25">
+        <v>279.32799999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>2500</v>
+      </c>
+      <c r="B26">
+        <v>845.23800000000006</v>
+      </c>
+      <c r="C26">
+        <v>522.63099999999997</v>
+      </c>
+      <c r="D26">
+        <v>319.846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ember is the champ!
</commit_message>
<xml_diff>
--- a/stats/stats.xlsx
+++ b/stats/stats.xlsx
@@ -264,94 +264,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>3.66687899999669</c:v>
+                  <c:v>2.29023400000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.95758799999021</c:v>
+                  <c:v>4.54944200000318</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.2721729999902</c:v>
+                  <c:v>6.8264019999915</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.2921189999906</c:v>
+                  <c:v>9.09822699999495</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.3556639999878</c:v>
+                  <c:v>11.3923329999961</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.5766259999945</c:v>
+                  <c:v>13.7014930000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.0655819999956</c:v>
+                  <c:v>16.0234329999948</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33.8288309999916</c:v>
+                  <c:v>18.3126649999903</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>38.7615779999905</c:v>
+                  <c:v>20.6513169999961</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44.343241999988</c:v>
+                  <c:v>22.944239999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49.967816999997</c:v>
+                  <c:v>25.2865619999938</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55.9188789999898</c:v>
+                  <c:v>27.6265859999984</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>62.28180099999</c:v>
+                  <c:v>29.9653560000006</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>69.2907699999923</c:v>
+                  <c:v>32.4098299999896</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>76.7077999999892</c:v>
+                  <c:v>34.8912069999933</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>85.3721409999998</c:v>
+                  <c:v>37.4611769999901</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>94.3843229999911</c:v>
+                  <c:v>39.9626439999992</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>103.840688999989</c:v>
+                  <c:v>42.508680999992</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>113.868644999995</c:v>
+                  <c:v>45.137189999994</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>124.574116999996</c:v>
+                  <c:v>47.8311390000017</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>135.377866999988</c:v>
+                  <c:v>50.5881769999978</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>146.358882999993</c:v>
+                  <c:v>53.3732619999937</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>157.728696999998</c:v>
+                  <c:v>56.2058109999925</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>169.377899999992</c:v>
+                  <c:v>59.1130160000029</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>181.61981399999</c:v>
+                  <c:v>62.0811759999924</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>194.088393999991</c:v>
+                  <c:v>65.0537489999987</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>206.793086999998</c:v>
+                  <c:v>68.1051719999959</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>220.086448999994</c:v>
+                  <c:v>71.249364999996</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>233.409555999998</c:v>
+                  <c:v>74.4522969999961</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>246.886327</c:v>
+                  <c:v>77.7487009999895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -984,11 +984,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2088971688"/>
-        <c:axId val="2123973400"/>
+        <c:axId val="2122381016"/>
+        <c:axId val="2122374072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2088971688"/>
+        <c:axId val="2122381016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1017,7 +1017,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123973400"/>
+        <c:crossAx val="2122374072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1025,7 +1025,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123973400"/>
+        <c:axId val="2122374072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,7 +1055,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088971688"/>
+        <c:crossAx val="2122381016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1437,7 +1437,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1461,7 +1461,7 @@
         <v>100</v>
       </c>
       <c r="B2" s="1">
-        <v>3.66687899999669</v>
+        <v>2.2902340000000501</v>
       </c>
       <c r="C2">
         <v>2.3059680000005698</v>
@@ -1479,7 +1479,7 @@
         <v>200</v>
       </c>
       <c r="B3" s="1">
-        <v>7.9575879999902099</v>
+        <v>4.5494420000031797</v>
       </c>
       <c r="C3">
         <v>4.6888949999993201</v>
@@ -1497,7 +1497,7 @@
         <v>300</v>
       </c>
       <c r="B4" s="1">
-        <v>12.2721729999902</v>
+        <v>6.8264019999915</v>
       </c>
       <c r="C4">
         <v>7.2121340000012397</v>
@@ -1515,7 +1515,7 @@
         <v>400</v>
       </c>
       <c r="B5" s="1">
-        <v>16.292118999990599</v>
+        <v>9.0982269999949494</v>
       </c>
       <c r="C5">
         <v>9.9168689999933104</v>
@@ -1533,7 +1533,7 @@
         <v>500</v>
       </c>
       <c r="B6" s="1">
-        <v>20.355663999987801</v>
+        <v>11.3923329999961</v>
       </c>
       <c r="C6">
         <v>12.815823999990201</v>
@@ -1551,7 +1551,7 @@
         <v>600</v>
       </c>
       <c r="B7" s="1">
-        <v>24.576625999994501</v>
+        <v>13.701493000000401</v>
       </c>
       <c r="C7">
         <v>15.940770000001001</v>
@@ -1569,7 +1569,7 @@
         <v>700</v>
       </c>
       <c r="B8" s="1">
-        <v>29.065581999995601</v>
+        <v>16.0234329999948</v>
       </c>
       <c r="C8">
         <v>19.286947000000499</v>
@@ -1587,7 +1587,7 @@
         <v>800</v>
       </c>
       <c r="B9" s="1">
-        <v>33.828830999991602</v>
+        <v>18.3126649999903</v>
       </c>
       <c r="C9">
         <v>22.859349999998798</v>
@@ -1605,7 +1605,7 @@
         <v>900</v>
       </c>
       <c r="B10" s="1">
-        <v>38.7615779999905</v>
+        <v>20.651316999996101</v>
       </c>
       <c r="C10">
         <v>26.530724999989602</v>
@@ -1623,7 +1623,7 @@
         <v>1000</v>
       </c>
       <c r="B11" s="1">
-        <v>44.343241999988003</v>
+        <v>22.944239999996999</v>
       </c>
       <c r="C11">
         <v>30.461471000002302</v>
@@ -1641,7 +1641,7 @@
         <v>1100</v>
       </c>
       <c r="B12" s="1">
-        <v>49.967816999996998</v>
+        <v>25.2865619999938</v>
       </c>
       <c r="C12">
         <v>34.6916879999917</v>
@@ -1659,7 +1659,7 @@
         <v>1200</v>
       </c>
       <c r="B13" s="1">
-        <v>55.918878999989801</v>
+        <v>27.626585999998401</v>
       </c>
       <c r="C13">
         <v>39.053764999989603</v>
@@ -1677,7 +1677,7 @@
         <v>1300</v>
       </c>
       <c r="B14" s="1">
-        <v>62.281800999989997</v>
+        <v>29.9653560000006</v>
       </c>
       <c r="C14">
         <v>43.638800999993599</v>
@@ -1695,7 +1695,7 @@
         <v>1400</v>
       </c>
       <c r="B15" s="1">
-        <v>69.290769999992307</v>
+        <v>32.409829999989597</v>
       </c>
       <c r="C15">
         <v>48.528304999999797</v>
@@ -1713,7 +1713,7 @@
         <v>1500</v>
       </c>
       <c r="B16" s="1">
-        <v>76.707799999989206</v>
+        <v>34.891206999993301</v>
       </c>
       <c r="C16">
         <v>53.624559999996499</v>
@@ -1731,7 +1731,7 @@
         <v>1600</v>
       </c>
       <c r="B17" s="1">
-        <v>85.3721409999998</v>
+        <v>37.461176999990101</v>
       </c>
       <c r="C17">
         <v>58.959447000000999</v>
@@ -1749,7 +1749,7 @@
         <v>1700</v>
       </c>
       <c r="B18" s="1">
-        <v>94.384322999991099</v>
+        <v>39.962643999999202</v>
       </c>
       <c r="C18">
         <v>64.733485999997299</v>
@@ -1767,7 +1767,7 @@
         <v>1800</v>
       </c>
       <c r="B19" s="1">
-        <v>103.840688999989</v>
+        <v>42.508680999992002</v>
       </c>
       <c r="C19">
         <v>70.506054999990695</v>
@@ -1785,7 +1785,7 @@
         <v>1900</v>
       </c>
       <c r="B20" s="1">
-        <v>113.868644999995</v>
+        <v>45.137189999994</v>
       </c>
       <c r="C20">
         <v>76.481748999998601</v>
@@ -1803,7 +1803,7 @@
         <v>2000</v>
       </c>
       <c r="B21" s="1">
-        <v>124.57411699999599</v>
+        <v>47.831139000001698</v>
       </c>
       <c r="C21">
         <v>82.745977999991695</v>
@@ -1821,7 +1821,7 @@
         <v>2100</v>
       </c>
       <c r="B22" s="1">
-        <v>135.37786699998799</v>
+        <v>50.588176999997799</v>
       </c>
       <c r="C22">
         <v>89.393891999992704</v>
@@ -1839,7 +1839,7 @@
         <v>2200</v>
       </c>
       <c r="B23" s="1">
-        <v>146.358882999993</v>
+        <v>53.373261999993701</v>
       </c>
       <c r="C23">
         <v>96.178527999989399</v>
@@ -1857,7 +1857,7 @@
         <v>2300</v>
       </c>
       <c r="B24" s="1">
-        <v>157.72869699999799</v>
+        <v>56.205810999992501</v>
       </c>
       <c r="C24">
         <v>103.23743399999501</v>
@@ -1875,7 +1875,7 @@
         <v>2400</v>
       </c>
       <c r="B25" s="1">
-        <v>169.377899999992</v>
+        <v>59.113016000002901</v>
       </c>
       <c r="C25">
         <v>110.614707</v>
@@ -1893,7 +1893,7 @@
         <v>2500</v>
       </c>
       <c r="B26" s="1">
-        <v>181.61981399998999</v>
+        <v>62.081175999992404</v>
       </c>
       <c r="C26">
         <v>118.093577999999</v>
@@ -1911,7 +1911,7 @@
         <v>2600</v>
       </c>
       <c r="B27" s="1">
-        <v>194.08839399999101</v>
+        <v>65.053748999998703</v>
       </c>
       <c r="C27">
         <v>125.925954999998</v>
@@ -1929,7 +1929,7 @@
         <v>2700</v>
       </c>
       <c r="B28" s="1">
-        <v>206.793086999998</v>
+        <v>68.105171999995903</v>
       </c>
       <c r="C28">
         <v>134.008726999993</v>
@@ -1947,7 +1947,7 @@
         <v>2800</v>
       </c>
       <c r="B29" s="1">
-        <v>220.08644899999399</v>
+        <v>71.249364999996004</v>
       </c>
       <c r="C29">
         <v>142.39921199998901</v>
@@ -1965,7 +1965,7 @@
         <v>2900</v>
       </c>
       <c r="B30" s="1">
-        <v>233.40955599999799</v>
+        <v>74.452296999996094</v>
       </c>
       <c r="C30">
         <v>151.000535999992</v>
@@ -1983,7 +1983,7 @@
         <v>3000</v>
       </c>
       <c r="B31" s="1">
-        <v>246.88632699999999</v>
+        <v>77.748700999989495</v>
       </c>
       <c r="C31">
         <v>159.932589999996</v>

</xml_diff>